<commit_message>
working on protocol 3
</commit_message>
<xml_diff>
--- a/fmt_2022_results.xlsx
+++ b/fmt_2022_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="288">
   <si>
     <t xml:space="preserve">day</t>
   </si>
@@ -387,7 +387,10 @@
     <t xml:space="preserve">Муковозчик</t>
   </si>
   <si>
-    <t xml:space="preserve">?</t>
+    <t xml:space="preserve">Серов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Карпенко</t>
   </si>
   <si>
     <t xml:space="preserve">Искалиев Андрей</t>
@@ -465,13 +468,46 @@
     <t xml:space="preserve">sum</t>
   </si>
   <si>
+    <t xml:space="preserve">ст1</t>
+  </si>
+  <si>
     <t xml:space="preserve">2:0</t>
   </si>
   <si>
+    <t xml:space="preserve">ст3</t>
+  </si>
+  <si>
     <t xml:space="preserve">1:1</t>
   </si>
   <si>
     <t xml:space="preserve">0:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ст9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ст4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ст2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ст5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ст6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ст7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ст11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ст8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ст10</t>
   </si>
   <si>
     <t xml:space="preserve">ВК</t>
@@ -930,12 +966,18 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FF99CCFF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1012,7 +1054,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1045,11 +1087,23 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="24" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="24" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1083,6 +1137,66 @@
     <cellStyle name="Result2" xfId="23"/>
     <cellStyle name="Excel Built-in Normal" xfId="24"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFAFD095"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1097,7 +1211,7 @@
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.41015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="10.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.73"/>
@@ -2199,11 +2313,11 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E54" activeCellId="0" sqref="E54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="15.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="15.79"/>
@@ -2313,6 +2427,9 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
@@ -2324,6 +2441,9 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>51</v>
       </c>
@@ -2781,9 +2901,6 @@
       <c r="D41" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -2793,13 +2910,10 @@
         <v>32</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D42" s="1" t="n">
         <v>2</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2815,9 +2929,6 @@
       <c r="D43" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
@@ -2827,7 +2938,7 @@
         <v>19</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D44" s="1" t="n">
         <v>2</v>
@@ -2841,7 +2952,7 @@
         <v>19</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D45" s="1" t="n">
         <v>2</v>
@@ -2855,7 +2966,7 @@
         <v>19</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D46" s="1" t="n">
         <v>1</v>
@@ -2869,7 +2980,7 @@
         <v>32</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D47" s="1" t="n">
         <v>1</v>
@@ -2925,7 +3036,7 @@
         <v>11</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D51" s="1" t="n">
         <v>2</v>
@@ -2939,7 +3050,7 @@
         <v>11</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D52" s="1" t="n">
         <v>2</v>
@@ -2953,7 +3064,7 @@
         <v>51</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D53" s="1" t="n">
         <v>2</v>
@@ -2981,7 +3092,7 @@
         <v>51</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D55" s="1" t="n">
         <v>2</v>
@@ -2995,7 +3106,7 @@
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D56" s="1" t="n">
         <v>1</v>
@@ -3009,7 +3120,7 @@
         <v>40</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D57" s="1" t="n">
         <v>2</v>
@@ -3023,7 +3134,7 @@
         <v>23</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D58" s="1" t="n">
         <v>1</v>
@@ -3037,7 +3148,7 @@
         <v>23</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D59" s="1" t="n">
         <v>2</v>
@@ -3051,7 +3162,7 @@
         <v>40</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D60" s="1" t="n">
         <v>1</v>
@@ -3177,7 +3288,7 @@
         <v>48</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D69" s="1" t="n">
         <v>2</v>
@@ -3191,7 +3302,7 @@
         <v>48</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D70" s="1" t="n">
         <v>1</v>
@@ -3205,7 +3316,7 @@
         <v>48</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D71" s="1" t="n">
         <v>1</v>
@@ -3247,7 +3358,7 @@
         <v>28</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D74" s="1" t="n">
         <v>2</v>
@@ -3261,7 +3372,7 @@
         <v>28</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D75" s="1" t="n">
         <v>2</v>
@@ -3275,7 +3386,7 @@
         <v>28</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D76" s="1" t="n">
         <v>2</v>
@@ -3303,7 +3414,7 @@
         <v>43</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D78" s="1" t="n">
         <v>1</v>
@@ -3317,7 +3428,7 @@
         <v>12</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D79" s="1" t="n">
         <v>1</v>
@@ -3331,7 +3442,7 @@
         <v>12</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D80" s="1" t="n">
         <v>1</v>
@@ -3345,7 +3456,7 @@
         <v>12</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D81" s="1" t="n">
         <v>1</v>
@@ -3359,7 +3470,7 @@
         <v>19</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D82" s="1" t="n">
         <v>1</v>
@@ -3373,7 +3484,7 @@
         <v>19</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D83" s="1" t="n">
         <v>2</v>
@@ -3387,7 +3498,7 @@
         <v>19</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D84" s="1" t="n">
         <v>1</v>
@@ -3443,7 +3554,7 @@
         <v>19</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D88" s="1" t="n">
         <v>2</v>
@@ -3513,7 +3624,7 @@
         <v>39</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D93" s="1" t="n">
         <v>2</v>
@@ -3527,7 +3638,7 @@
         <v>39</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D94" s="1" t="n">
         <v>1</v>
@@ -3541,7 +3652,7 @@
         <v>39</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D95" s="1" t="n">
         <v>1</v>
@@ -3569,7 +3680,7 @@
         <v>35</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D97" s="1" t="n">
         <v>2</v>
@@ -3583,7 +3694,7 @@
         <v>44</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D98" s="1" t="n">
         <v>2</v>
@@ -3597,7 +3708,7 @@
         <v>44</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D99" s="1" t="n">
         <v>2</v>
@@ -3611,7 +3722,7 @@
         <v>44</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D100" s="1" t="n">
         <v>1</v>
@@ -3625,7 +3736,7 @@
         <v>44</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D101" s="1" t="n">
         <v>1</v>
@@ -3879,11 +3990,11 @@
   </sheetPr>
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y12" activeCellId="0" sqref="Y12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.41015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="6.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.79"/>
@@ -3895,6 +4006,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="7.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="19" style="0" width="3.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="7.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="24" style="8" width="10.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3964,21 +4076,25 @@
       <c r="W1" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="X1" s="0" t="s">
-        <v>145</v>
+      <c r="X1" s="9" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="B2" s="10"/>
+      <c r="E2" s="0" t="s">
+        <v>147</v>
+      </c>
       <c r="H2" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="X2" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="X2" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -3986,13 +4102,17 @@
       <c r="A3" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="C3" s="10"/>
       <c r="F3" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>149</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="X3" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="X3" s="9" t="n">
         <v>3</v>
       </c>
     </row>
@@ -4000,13 +4120,17 @@
       <c r="A4" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="D4" s="10"/>
       <c r="H4" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>152</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="X4" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="X4" s="9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4014,13 +4138,17 @@
       <c r="A5" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="B5" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="10"/>
       <c r="O5" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="X5" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="X5" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -4029,12 +4157,16 @@
         <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="P6" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="P6" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="X6" s="0" t="n">
+      <c r="U6" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="X6" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -4042,13 +4174,17 @@
       <c r="A7" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="G7" s="10"/>
+      <c r="I7" s="0" t="s">
+        <v>154</v>
+      </c>
       <c r="N7" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="V7" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="X7" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="X7" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -4057,12 +4193,16 @@
         <v>40</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="X8" s="0" t="n">
+      <c r="H8" s="10"/>
+      <c r="J8" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="X8" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -4070,13 +4210,17 @@
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="G9" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="I9" s="10"/>
       <c r="J9" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="X9" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="X9" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -4084,13 +4228,17 @@
       <c r="A10" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="H10" s="0" t="s">
+        <v>155</v>
+      </c>
       <c r="I10" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="T10" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="T10" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="X10" s="0" t="n">
+      <c r="X10" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -4098,13 +4246,17 @@
       <c r="A11" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="K11" s="10"/>
       <c r="L11" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>156</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="X11" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="X11" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -4113,12 +4265,16 @@
         <v>44</v>
       </c>
       <c r="K12" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="L12" s="10"/>
+      <c r="O12" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="V12" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="V12" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="X12" s="0" t="n">
+      <c r="X12" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -4127,12 +4283,16 @@
         <v>27</v>
       </c>
       <c r="I13" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="M13" s="10"/>
+      <c r="T13" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="T13" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="X13" s="0" t="n">
+      <c r="X13" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -4140,13 +4300,17 @@
       <c r="A14" s="0" t="s">
         <v>48</v>
       </c>
+      <c r="D14" s="0" t="s">
+        <v>152</v>
+      </c>
       <c r="G14" s="0" t="s">
-        <v>148</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="N14" s="10"/>
       <c r="Q14" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="X14" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="X14" s="9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4155,13 +4319,17 @@
         <v>28</v>
       </c>
       <c r="E15" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="N15" s="11"/>
+      <c r="O15" s="10"/>
+      <c r="W15" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="N15" s="8"/>
-      <c r="W15" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="X15" s="0" t="n">
+      <c r="X15" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -4170,12 +4338,16 @@
         <v>43</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>148</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="P16" s="10"/>
       <c r="R16" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="X16" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="T16" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="X16" s="9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4183,13 +4355,17 @@
       <c r="A17" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="C17" s="0" t="s">
+        <v>149</v>
+      </c>
       <c r="K17" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="X17" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="Q17" s="10"/>
+      <c r="X17" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -4198,12 +4374,16 @@
         <v>32</v>
       </c>
       <c r="E18" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="P18" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="P18" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="X18" s="0" t="n">
+      <c r="R18" s="10"/>
+      <c r="S18" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="X18" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -4212,12 +4392,16 @@
         <v>51</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="X19" s="0" t="n">
+      <c r="R19" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="S19" s="10"/>
+      <c r="X19" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -4226,12 +4410,16 @@
         <v>35</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="X20" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="T20" s="10"/>
+      <c r="X20" s="9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4240,12 +4428,16 @@
         <v>20</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>147</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="U21" s="10"/>
       <c r="W21" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="X21" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="X21" s="9" t="n">
         <v>3</v>
       </c>
     </row>
@@ -4254,12 +4446,16 @@
         <v>47</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="X22" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="V22" s="10"/>
+      <c r="W22" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="X22" s="9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4268,12 +4464,16 @@
         <v>52</v>
       </c>
       <c r="O23" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="U23" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="X23" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="V23" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="W23" s="10"/>
+      <c r="X23" s="9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4299,7 +4499,7 @@
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.41015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.09"/>
   </cols>
@@ -4336,27 +4536,27 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4391,7 +4591,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4445,19 +4645,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="4" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4470,7 +4670,7 @@
         <v>29</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>31</v>
@@ -4486,7 +4686,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>19</v>
@@ -4499,10 +4699,10 @@
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>23</v>
@@ -4518,7 +4718,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>23</v>
@@ -4528,13 +4728,13 @@
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>162</v>
+      <c r="B6" s="12" t="s">
+        <v>174</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>19</v>
@@ -4550,7 +4750,7 @@
         <v>25</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>11</v>
@@ -4566,7 +4766,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>12</v>
@@ -4582,7 +4782,7 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>24</v>
@@ -4598,7 +4798,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>40</v>
@@ -4614,7 +4814,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>39</v>
@@ -4630,7 +4830,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>16</v>
@@ -4646,7 +4846,7 @@
         <v>22</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>16</v>
@@ -4662,7 +4862,7 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>44</v>
@@ -4678,7 +4878,7 @@
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>27</v>
@@ -4694,7 +4894,7 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>48</v>
@@ -4710,7 +4910,7 @@
         <v>74</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>28</v>
@@ -4726,7 +4926,7 @@
         <v>72</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>28</v>
@@ -4742,7 +4942,7 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>43</v>
@@ -4758,7 +4958,7 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>36</v>
@@ -4774,7 +4974,7 @@
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>32</v>
@@ -4790,7 +4990,7 @@
         <v>42</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>51</v>
@@ -4801,12 +5001,12 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>35</v>
@@ -4822,7 +5022,7 @@
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>20</v>
@@ -4838,7 +5038,7 @@
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>47</v>
@@ -4854,7 +5054,7 @@
         <v>50</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>52</v>
@@ -4870,7 +5070,7 @@
         <v>41</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F27" s="4"/>
     </row>
@@ -4884,7 +5084,7 @@
         <v>45</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F28" s="4"/>
     </row>
@@ -4895,10 +5095,10 @@
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F29" s="4"/>
     </row>
@@ -4912,7 +5112,7 @@
         <v>53</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F30" s="4"/>
     </row>
@@ -4926,7 +5126,7 @@
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F31" s="4"/>
     </row>
@@ -4939,7 +5139,7 @@
         <v>55</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="F32" s="4"/>
     </row>
@@ -4948,7 +5148,7 @@
         <v>69</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -4985,237 +5185,237 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="A1" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H2" s="4" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>173</v>
+      <c r="A3" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>175</v>
+      <c r="A4" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>187</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="G4" s="4" t="n">
         <v>2</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>179</v>
+      <c r="A5" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>191</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="G5" s="4" t="n">
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>182</v>
+      <c r="A6" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>194</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="G6" s="4" t="n">
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>186</v>
+      <c r="A7" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>198</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="G7" s="4" t="n">
         <v>2</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>190</v>
+      <c r="A8" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>202</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="G8" s="4" t="n">
         <v>2</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>194</v>
+      <c r="A9" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>206</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="G9" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>199</v>
+      <c r="A10" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>211</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="G10" s="4" t="n">
         <v>2</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>203</v>
+      <c r="A11" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>215</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="G11" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>209</v>
+      <c r="A12" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>221</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>38</v>
@@ -5225,51 +5425,51 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="G12" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>213</v>
+      <c r="A13" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>225</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="G13" s="4" t="n">
         <v>1</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>217</v>
+      <c r="A14" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>229</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6" t="s">
@@ -5280,46 +5480,46 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>221</v>
+      <c r="A15" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>233</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>34</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="G15" s="4" t="n">
         <v>1</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>225</v>
+      <c r="A16" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>237</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6" t="s">
@@ -5330,11 +5530,11 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>229</v>
+      <c r="A17" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>241</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>37</v>
@@ -5344,30 +5544,30 @@
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="G17" s="4" t="n">
         <v>1</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>232</v>
+      <c r="A18" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>244</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6" t="s">
@@ -5378,17 +5578,17 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>236</v>
+      <c r="A19" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>248</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6" t="s">
@@ -5399,110 +5599,110 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>240</v>
+      <c r="A20" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>252</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="G20" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>244</v>
+      <c r="A21" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>256</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="4" t="n">
         <v>2</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>248</v>
+      <c r="A22" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>260</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="G22" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>252</v>
+      <c r="A23" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>264</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="G23" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>256</v>
+      <c r="A24" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>268</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6" t="s">
@@ -5513,27 +5713,27 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>260</v>
+      <c r="A25" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>272</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="G25" s="4" t="n">
         <v>2</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5544,7 +5744,7 @@
         <v>2</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5555,7 +5755,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5566,7 +5766,7 @@
         <v>2</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5577,7 +5777,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5588,18 +5788,18 @@
         <v>1</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="4" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="G31" s="4" t="n">
         <v>1</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5628,7 +5828,7 @@
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="3" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5645,7 +5845,7 @@
         <v>14</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5662,7 +5862,7 @@
         <v>18</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5679,7 +5879,7 @@
         <v>22</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5696,7 +5896,7 @@
         <v>26</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5713,7 +5913,7 @@
         <v>30</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5730,7 +5930,7 @@
         <v>34</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5747,7 +5947,7 @@
         <v>38</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5764,7 +5964,7 @@
         <v>42</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5781,7 +5981,7 @@
         <v>46</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5798,7 +5998,7 @@
         <v>50</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5815,7 +6015,7 @@
         <v>54</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>